<commit_message>
Adding i want page
</commit_message>
<xml_diff>
--- a/RR/excel/Run_Script.xlsx
+++ b/RR/excel/Run_Script.xlsx
@@ -96,7 +96,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +108,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -576,137 +584,145 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1031,7 +1047,7 @@
   <dimension ref="A2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1049,6 +1065,7 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="2"/>
       <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1060,6 +1077,7 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F3" s="3"/>
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1086,7 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1078,22 +1096,23 @@
       </c>
     </row>
     <row r="6" spans="8:8">
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="8:8">
+    <row r="7" spans="5:8">
+      <c r="E7" s="5"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="8:8">
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="8:8">
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1128,7 +1147,7 @@
       </c>
     </row>
     <row r="21" ht="28.8" spans="1:2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1136,6 +1155,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="dheerajc@advantageclub.in"/>
     <hyperlink ref="B12" r:id="rId2" display="Dheeraj@4321"/>

</xml_diff>